<commit_message>
Development Of new project an for done
</commit_message>
<xml_diff>
--- a/JainSanghInformation/excelfile/MemberMaster.xlsx
+++ b/JainSanghInformation/excelfile/MemberMaster.xlsx
@@ -1,40 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C387263A-59F8-4EE0-B351-0CD18B942F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72F9ADF-0D40-409C-BD27-C740FBBC9752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$4</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>Birthdate</t>
   </si>
@@ -60,61 +54,70 @@
     <t>MobileNumberSecondary</t>
   </si>
   <si>
-    <t>The Bharuch Jila Ladua Shrimali Sw. Mu. Jain Sangh-Valsad, Navsari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Self </t>
-  </si>
-  <si>
     <t>Son</t>
   </si>
   <si>
     <t>Wife</t>
   </si>
   <si>
-    <t>Upesh Ratilal shah</t>
-  </si>
-  <si>
-    <t>Manisha Upesh shah</t>
-  </si>
-  <si>
-    <t>Kevin Upesh shah</t>
-  </si>
-  <si>
-    <t>18/11/1967</t>
-  </si>
-  <si>
-    <t>19/05/1999</t>
-  </si>
-  <si>
-    <t>8-pass</t>
-  </si>
-  <si>
-    <t>B.com</t>
-  </si>
-  <si>
-    <t>12+ItI -pass</t>
-  </si>
-  <si>
     <t>Married</t>
   </si>
   <si>
-    <t>unmarried</t>
-  </si>
-  <si>
-    <t>Job</t>
-  </si>
-  <si>
-    <t>House-Wife</t>
-  </si>
-  <si>
-    <t>Ankleshwar</t>
-  </si>
-  <si>
-    <t>507, Siddharth apt, sandkuva ,new police station, Navsari,396445</t>
-  </si>
-  <si>
     <t>B+</t>
+  </si>
+  <si>
+    <t>NativePlace</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Occupation Address</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>Amitbhai Bipinchnadra Shah</t>
+  </si>
+  <si>
+    <t>Amitbhai Bipinchndra Shah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monikaben Amitbhai Shah </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev Amitbhai Shah </t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Unmarried</t>
+  </si>
+  <si>
+    <t>B-33, Saarthi Apartment, Bh.Avishkar Tenament, Ghatlodiya, Ahmedabad, Gujarat-380061</t>
+  </si>
+  <si>
+    <t>O+</t>
+  </si>
+  <si>
+    <t>amitshah97256@gmail.com</t>
+  </si>
+  <si>
+    <t>monikashah111171@gmail.com</t>
+  </si>
+  <si>
+    <t>devshah17112002@gmail.com</t>
+  </si>
+  <si>
+    <t>B.Com</t>
   </si>
   <si>
     <r>
@@ -123,7 +126,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Cambria"/>
         <family val="1"/>
@@ -138,7 +141,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Cambria"/>
         <family val="1"/>
@@ -153,7 +156,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Cambria"/>
         <family val="1"/>
@@ -168,7 +171,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Cambria"/>
         <family val="1"/>
@@ -177,7 +180,28 @@
     </r>
   </si>
   <si>
-    <t>NativePlace</t>
+    <r>
+      <t>Gender</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Anand</t>
+  </si>
+  <si>
+    <t>Ahmedabad</t>
+  </si>
+  <si>
+    <t>Bardoli</t>
   </si>
 </sst>
 </file>
@@ -185,9 +209,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-7000447]0"/>
+    <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,23 +220,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9.35"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Cambria"/>
       <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -247,26 +296,57 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -325,7 +405,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -360,7 +440,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -545,187 +625,224 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="1" customWidth="1"/>
+    <col min="11" max="11" width="111.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="73.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="5"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="10">
+        <v>24655</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="4">
+        <v>9725366323</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="10">
+        <v>26248</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="4">
+        <v>9998902113</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="10">
+        <v>37577</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="4">
+        <v>8401912391</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="2">
-        <v>8690990459</v>
-      </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="5">
-        <v>26149</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="2">
-        <v>9998338960</v>
-      </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="126" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="3">
-        <v>8735843814</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="P3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="P4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>